<commit_message>
Get daily reddit data: Tue Jul  2 08:09:25 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_07.xlsx
+++ b/data/2024_07_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C491"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,3236 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1dtg4eb</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Random diy :3</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtg4eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1dtg3o5</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Recent set done by my 16 yr old sister</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtg3o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1dtg2de</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Actual question/curiosity for those who…</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtg2de/actual_questioncuriosity_for_those_who/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1dtfuj3</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>I sigh in admiration looking at my beautiful nails</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g4s01mds32ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1dtf6wj</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Best Options for Oily Nail Bed</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtf6wj/best_options_for_oily_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1dteo63</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got my dream nails!!  </t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wni3c8qp1ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1dtecaa</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>First attempt at painted nail art. What do you think?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtecaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1dte82x</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Relaxing and did my nails</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dte82x</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1dte4jz</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Name for the Nail Salon</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dte4jz/name_for_the_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1dte1kg</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>RATE THE NAILSSS</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4krxv8di1ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1dte1fi</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Fourth of July Nails 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dte1fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1dte04w</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Silver nails</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94m7tj4xh1ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1dtdymi</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>4th of July</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29fjpyyfh1ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1dtdxfp</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Classy Hawaiian Print</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtdxfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1dtdiu5</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>First take at snoopy nails 💀</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8d8fzblc1ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1dtdi9d</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Too simple?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5695cidc1ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1dtdcmh</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>I love matching my Camaro! 😮‍💨 anyone else does this? 💚</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofu3klqoa1ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1dtdbso</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>My Ocean Themed Nails</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmgo1h9ga1ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1dtd88a</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy 4th! This set took me way too long, but it was worth it! </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drbrms8f91ad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1dtckck</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Lets say i paint my nails in a room with the doors closed does the smell get out of the room and into the living room/hall?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtckck/lets_say_i_paint_my_nails_in_a_room_with_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1dtcgbo</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>It’s been a minuteeee</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtcgbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1dtceef</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Halloween came early this year. Gel-x nails done by me 💚🖤</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtceef</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1dtcc63</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Bubbles !!! 🐸</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zx5ajbf01ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1dtbpgo</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>The way my nail girl tried to talk me out of pink and white…</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhl3baheu0ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1dtbow3</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>I want to do a design like this. These are by Lindsey Michelle, looks like.</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvbduox8u0ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1dtblwy</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>❤️🤍💙</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtblwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1dtb647</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel removal </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtb647</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1dtb06l</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>ISO: Phoenix East Valley Nail Techs</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtb06l/iso_phoenix_east_valley_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1dtalf7</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>A blue kinda Monday 😌</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtalf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1dtairm</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>First time painting my own nails!</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ju102wfj0ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1dta83u</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>4th of July nails. Press ons</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4h6ax2vg0ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1dt9v51</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Summer birthday nails!</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt9v51</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1dt9hp3</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Too wide?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt9hp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1dt9d0y</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>I just discovered the GREATEST nail hack!</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dt9d0y/i_just_discovered_the_greatest_nail_hack/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1dt9b3m</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Just made my first ever set of press ons</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/io9e5ruj80ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1dt92sw</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Need some help</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dt92sw/need_some_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1dt90vk</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Happy 4th! ❤️🤍💙</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bjnhaz260ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1dt8io2</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">jeans and nudes </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmg9fy8m10ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1dt844n</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Inspired by Clase Azul + my 1st time with almond instead of square</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgtdfbb5yz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1dt80lx</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Reptar nails 🦖</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcd4otydxz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1dt7zk5</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Love themm</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfgk03u4xz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1dt7mr0</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>C-shaped Nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2a8w9506uz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1dt7hwg</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Sparkly Claws</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzzoss91tz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1dt79ri</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Really bad picture, but do these look weird to anyone else? It's my first time getting long press ons.</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxln85ywqz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1dt74x1</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>My 4th of july design!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt74x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1dt6zvb</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Wanted a kind of beachy theme</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzmbhd2xoz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1dt6yzb</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>I tried some stickers ✨✨</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzk4lsvpoz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1dt6win</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Been getting the same ombré for a long time, I just can’t get sick of this style</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvzdkrx5oz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1dt6rp1</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Cat eye</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yt0dy33nz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1dt67oc</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Best nail extension tips for making press-ons with small nail buds?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dt67oc/best_nail_extension_tips_for_making_pressons_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1dt65gq</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Mexico Nails!</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt65gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1dt5zn6</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Hotdogs on my 4th July Nails</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww0fczdzgz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1dt59eq</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>ponyo !!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt59eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1dt653p</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>4th of July nails 💅</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0nsms85iz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1dt5zlw</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt5zlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1dt5s4i</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Violet frenchies &lt;3</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6usqxidfz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1dt5q1z</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>First DIY Gel Manicure</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwtmlujuez9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1dt5izd</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Do you ever just ignore the laws of physics and try anyway?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/03n7aoqfdz9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1dt5b99</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Matte pink!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mljw1sxubz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1dt55f2</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>First Time Doing Gel X Extensions !</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ei5sldmaz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1dt5004</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Nude with pearl chrome 🤗</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt5004</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1dt4icx</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Trouble shaping my nail</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt4icx</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1dt43qe</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">glitch nails tutorial </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/caigzo1b2z9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1dt41ul</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Did I find a good one in the wild?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jbkixz72z9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1dt3qg9</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Did I mention…they glow!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt3qg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1dt3psm</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Stay with coffin or go round?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt3psm</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1dt3mje</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Nail growth tips and tricks?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qeeryfb3zy9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1dt2u7y</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>How can I achieve this color? Inspo pic: @thisisvenice on IG</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9g8a5btdty9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1dt32ey</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of this nail length ? </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1z5eh5o0vy9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1dt2mmp</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Beach Nails with a 4th of July twist 🎊</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt2mmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1dt2iu0</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>tried to treat myself for my birthday and these are the worst I've paid for in a long time</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt2iu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1dt2gum</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Cloud nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt2gum</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1dt26xw</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Can I use polygel instead of acrylics?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dt26xw/can_i_use_polygel_instead_of_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1dt25ju</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Strawberry shortcake 🍓🍰</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt25ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1dt1yqs</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>What do I do? :(</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rto3kfh0ny9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1dt1sq8</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Help With Discontinued Colour</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt1sq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1dt1u2f</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>What is a fair price for gel on natural nails</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt1u2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1dt1sqa</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>I make custom press-ons🩵</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y666eyfqly9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1dt1lxj</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>So happy with my new nail tech</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt1lxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1dt1jia</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Trying to grow my natural nails. It’s going great</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ybjyb4vjy9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1dt17s2</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Need advice on acrylics</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dt17s2/need_advice_on_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1dt11xe</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>I really loved my wedding nails!</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6coopvagy9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1dt10n9</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Looking for dark plum pr dark berry press on nails</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dt10n9/looking_for_dark_plum_pr_dark_berry_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1dt0nir</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just finished doing my 4th of July nails </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt0nir</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1dt0mt5</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Getting better at painting my right hand! Constructive criticism please. I struggle the most with my cuticles!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt0mt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1dt0h6v</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Chameleon color ✨</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt0h6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1dt0h14</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>You look like the 4h of July. It makes me want a hotdog real bad</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt0h14</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1dszxke</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Sculpted stiletto, I loved them!❤</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqvn4jh88y9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1dszx2y</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Second set I have done, any tips appreciated</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dszx2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1dszv8p</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>My little nail journey</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dszv8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1dsd604</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>I hate my nails</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsd604</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1dsasxn</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Help! My nail tech ruined my nails, I did a removal, and need advice on if I should go all natural and let them heal or a clear/protective coat to help them heal?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8ljw09crr9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1dse9ak</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>June nails 🥰💅🏼</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dse9ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1dsf57c</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Technician used a tool on my cuticles and marked my nails…</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dsf57c/technician_used_a_tool_on_my_cuticles_and_marked/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1dslkmi</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>First time doing gel x ... I want to take them off already :(</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ag646bouiu9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1dsnma4</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first ever diy gel nails! </t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dsnma4/my_first_ever_diy_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1dsqxhy</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Best 'normal' polish brands that aren't Essie</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dsqxhy/best_normal_polish_brands_that_arent_essie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1dszce4</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Lots of rad nails this week ✨</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dszce4</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1dsz5hq</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>The length chart!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8p6keim2y9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1dsz59x</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>🤯</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo0ci16l2y9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1dtfaqp</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>The mooncat x powerpuff girls collab is everything my inner child ever wanted</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtfaqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1dtevsx</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>My favorite lavender jelly 💜</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtevsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1dtdyrp</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>La Bahía and You, of Unshakable Conviction</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtdyrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1dtd4bl</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>I have a type :)</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtd4bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1dtcnr7</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>This is your sign to get Sour Apple Rings in PPU Rewind 💚⚡️</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eww8pgwo31ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1dtav2c</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Berry style)</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mym4jhw7m0ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1dtao5z</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>A blue kinda Monday</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtao5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1dtamnz</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>4 days into this mani</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ejyiqndk0ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1dtalnp</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Painted my nails for the first time at 31</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytb74mm4k0ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1dtaa4d</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Hopping on the jade train💚</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtaa4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1dt9qyv</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Atomic Polish Narf 🤩</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt9qyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1dt98zb</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Any idea on what polish this could be?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nn7mtau480ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1dt9811</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Flower Child 🌷</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt9811</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1dt961a</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Custom polish from DragonSworn</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7609eld70ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1dt8rwo</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prugly? Just ugly? </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cm90p7w30ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1dt8ldi</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Not loving the NightGlo formula 🫠</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt8ldi</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1dt8fxz</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'll still talk trash but they have great colors </t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt8fxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1dt7p2j</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy 4th, and reminder to register to VOTE </t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt7p2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1dt7ny3</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Marbling with DVN!</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt7ny3</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1dt7hig</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Sugar, Spice and Everything Nice - KBShimmer</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt7hig</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1dt7gpj</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>4th of July nails</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt7gpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1dt6foa</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Looking for a gel version of this color, please!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt6foa</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1dt620k</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Cottage Manis</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt620k</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1dt5zvw</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Ditching creams - Going with Jellies</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dt5zvw/ditching_creams_going_with_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1dt5xq5</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>💅NAIL MAIL MONDAY💅</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kso3hlkgz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1dt5vvj</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Opaque builder gel?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dt5vvj/opaque_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1dt4s3y</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>First LynB order, not regretting branching out!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q02xl6ip7z9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1dt4oyz</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Take me back to spring and away from this heat</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt4oyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1dt4j73</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>My June shorties!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt4j73</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1dt3ryo</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Mooncat’s Maelstrom Has Me Emo Beach Ready 🖤🌴</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt3ryo</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1dt3dnd</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Wildflower Lacquer - Yippee Skippee💕</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt3dnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1dt2qh9</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque “Road Rage” </t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4d7tzlnksy9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1dt2cfn</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Rubber base gel under polish?</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dt2cfn/rubber_base_gel_under_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1dt22a3</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Matching jade nails</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt22a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1dt1zmn</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Another Phoenix (EDK) magnetic!</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt1zmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1dt1hsc</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Purple gray sparkles!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt1hsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1dt11px</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PFD limelight vs atomic sour apple rings </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dt11px/pfd_limelight_vs_atomic_sour_apple_rings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1dt0kq1</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Streaky polish fixes?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dt0kq1/streaky_polish_fixes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1dt071q</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Ethereal-Ether Dragon VS Polished for days-Lush</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt071q</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1dszo83</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>You guys put me onto Essie wicked 🖤</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t9350hc6y9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1dsyi0c</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>IL ❤️ ILNP!</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1muim8krxx9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1dsyhz3</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Press-ing question</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsyhz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1dsy6kf</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>How do I avoid getting bubbles/bumps on my nail polish?</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsy6kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1dsy5s2</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>PBE💅 + hibachi🍱 + la(c)queristas👯‍♀️ = can't lose</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dsy5s2/pbe_hibachi_lacqueristas_cant_lose/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1dsxvs3</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Christmas in July! (Xmas Sky by Vanessa Molina)</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsxvs3</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1dsxd7f</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>🙀❤️😍</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkz2raxgpx9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1dsx4vz</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Baja Blasted with Flower Power topp</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsx4vz</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1dsw77s</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Beginner Nail Art</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dsw77s/beginner_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1dsvvub</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Pretty basic but I’m in love 🖤</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vflzl9ppex9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1dsuu7d</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>BKL i was almost a pancake &amp; DVN tomb of wrestlers</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsuu7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1dsuhci</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Ether Dragon vs PFD Lush</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dsuhci/ether_dragon_vs_pfd_lush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1dsu4pn</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>why get new polish when old polish do trick</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsu4pn</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1dstyj4</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Lookalike?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dstyj4/lookalike/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1dstmpv</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>What are your top suggestions from Death Valley Nails indie brand?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dstmpv/what_are_your_top_suggestions_from_death_valley/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1dstm9z</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>What are your top suggestions from Death Valley Nails indie brand?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dstm9z/what_are_your_top_suggestions_from_death_valley/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1dstak5</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Palate cleanser but make it fun</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhn0uulcvw9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1dsslov</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>got my first russian mani (while trying to grow out my natural nails) 💅✨</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsslov</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1dssgjs</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>A surprising new favorite!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dssgjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1dss8cw</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>My mom couldn’t understand why I grew my natural nails so long until her manicurist did my nails and she finally saw my vision for my baby fingers.</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dss8cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1dss6dm</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>First home pedicure (male) . I Posted elsewhere and was advised i needed to prep before colour, i.e fix nail ridges et cetera, how do I fix this at home ? Thanks in advance.</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fl17umylw9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1dss12c</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Night Glo from Polished for Days</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dss12c</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1dsrgol</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Advice please. Why is this happening with my BIAB?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsrgol</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1dsr6j5</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Cuticula Limitless won't dry on me</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mpeq8xpcw9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1dsqijo</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>I hate my wedding manicure… Advice please!</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsqijo</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1dspae0</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dspae0/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1dspadn</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dspadn/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1dsoxfm</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Do I need Sour Apple Rings?</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wt2r7lvnv9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1dso3lb</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tfw the nail gods are against you </t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dso3lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1dtf4g1</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Cat eye nails</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4abl4fyu1ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1dtdz7p</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello! I just wanted to share my new nail euphoria somewhere! </t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dtdz7p/hello_i_just_wanted_to_share_my_new_nail_euphoria/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1dtcelo</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Who’s that Pokemon?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgn3ppc311ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1dtai1s</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>A detailed video on making nail art gel</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c6qrkjb2j0ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1dt7d1s</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Nail art polish</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dt7d1s/nail_art_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1dt6vpq</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Diamond Nails </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzeb28gznz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1dt6nut</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0blmg819mz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1dt6kn7</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>I needed a lot of effort to make this design, did you like the result?</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4eaqxa85lz9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1dt5yvl</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>glitch nails tutorial!!</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://vm.tiktok.com/ZMrhn557L/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1dt4hq8</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Bulky gel</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dt4hq8/bulky_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1dt3yod</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cutes </t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93ulucbl1z9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1dt13qf</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Aura Nails look bad and patchy :(</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alj4drpogy9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1dt0d7c</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>My first 3D -ish paint job</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dt0d7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1dszpwp</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">aquarium nails </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dszpwp/aquarium_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1dsyc3f</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Simple but cute</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzg05h9jwx9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1dsxh9l</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>What nail tips do you recommend?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dsxh9l/what_nail_tips_do_you_recommend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1dsx1xh</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>I'm creating a Bobs burgers press on nail set for fun✨ here's Linda and gene with a 3d mustard bottle 🙌🤩</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1qtv6wu4nx9d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1dsvljc</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Do you like to use aurora effect?💜</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iysinmoocx9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1dsv8nt</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Matching</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dsv8nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1dstyw2</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>DIY Biab, loving this cute little heart!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0otj925p0x9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1dsr7ur</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hey all I was just looking some friendly advice on how to improve my free edge 💅🫶 </t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujz92he3dw9d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1dsnoy7</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>"Let's summarize the nail sets I've done over the past few days."</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9hurpmc8v9d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jul  3 08:09:18 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_07.xlsx
+++ b/data/2024_07_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C491"/>
+  <dimension ref="A1:C684"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8781,6 +8781,3287 @@
         </is>
       </c>
     </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1du8ypi</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What can I do to make them appear broader,I feel hard to practice any nail art on these </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2tcbply4g9ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1du8pi6</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>New Set New Tech</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92zwlzwtc9ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1du7yk2</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>cat eye nails!!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fatjgn7q39ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1du7sze</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Many hours later, here are my nails I did myself</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du7sze</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1du725p</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>I (M29) am having a daughter in August. I wanna get my nails done and know nothing.</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1du725p/i_m29_am_having_a_daughter_in_august_i_wanna_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1du6oi8</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>💕</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2agksviuo8ad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1du6gia</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why would my nail bed randomly separate from my nail? The middle and ring finger both randomly started separated. </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du6gia</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1du61qi</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>this type of nails is out of fashion?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lbmosp3i8ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1du5wo9</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>I love jello jello one kill base coat and remover</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/115bkyukg8ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1du5ovp</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Butterfly nails I did!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b2o0k8u7e8ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1du5j8o</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>4th of July nails 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wuez0emc8ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1du5hz8</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done for the first time ever, and I love it! </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzal8639c8ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1du5gg9</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>4th of July nails</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du5gg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1du5beh</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Long time biter transformed by biab in five weeks!!!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du5beh</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1du59e5</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Loooook😘 I did myself💅🏼</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du59e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1du52gl</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>First set of the summer 🩵🍊</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hr2fkicy78ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1du43lu</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Color design, what do you think?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu8pgx6iy7ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1du3v2a</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Impress nails-sticky residue help</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1du3v2a/impress_nailssticky_residue_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1du3tv9</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>A little late, but I got my pride nails! 💙💜🩷</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7dtzaoyv7ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1du3t57</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>I found better lighting, also introducing my other hand</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du3t57</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1du39rz</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Would you cut it off or buy nail glue? 😭</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9lxo7jqq7ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1du2o5m</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>[I'M A BOY] Some nails I did for myself last month to test out some polishes I got. This set is inspired by my favorite band, Caravan Palace; each nail has a color from 1 of their 5 albums. &lt;|^_^|&gt;</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du2o5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1du2y0w</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>My first fruit set! I’m obsessed 😍</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du2y0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1du2swy</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Lisa frank nails!</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du2swy</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1du2j2j</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>freshies 🎀</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k79ixoeyj7ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1du2j1o</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Love them!! For my cosplays this weekend</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p8munjyj7ad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1du2i7x</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brand new set! </t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcyc78wqj7ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1du2dpo</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>mocha summer~  ♡✿</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du2dpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1du2beo</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>AMERICA ❤️</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du2beo</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1du24rf</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer nails 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du24rf</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1du21v7</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>my fourth of july nails! 💅</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du21v7</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1du1tp5</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Did my first nail art! I made it Ukraine/Anti-war themed What do you think?)</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46cg5e0hd7ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1du1kmz</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Asked my husband to pick my new nail color</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du1kmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1du1hk2</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Hand painted my own nails for the Eras Tour!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcgzbwcka7ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1du1aly</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Natural nails are almost as long as my acrylics 💅</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phdqoc5t87ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1du16wz</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Marbly nails</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zdmojmw77ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1du15rg</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Update IV added Bob to the set! I'm debating doing a 3d cut up credit card for his nail that Louise made him 🥴🤣 if I had space I'd have the burger of the day on a board 😭</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/avnats9m77ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1du14cy</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Last few sets!! Love them all</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du14cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1du0zwn</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Cute press ons by me 🥰</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkvx4t2667ad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1du0qsb</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>New press on</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gueszrvz37ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1du0m6w</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Simple but patriotic</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmt2znnv27ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1du08c3</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Ponyo-inspired nails ☺️</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du08c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1du0he6</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>under da sea🐚</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du0he6</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1du0h9s</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Some fun black acrylics I did today :)</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mud3mr1q17ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1du04m8</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>My take on cherry nail art</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du04m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1du0365</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>First time painting hibiscus flowers 🌺</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du0365</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1dtzzua</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtzzua</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1dtzw2w</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Did a little 3d design to this set, i actually really like these with the little rainbow nail i did🥹</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtzw2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1dtzu62</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>My nails by @freaky_fresh_phalanges on insta vs the inspo (pic 3) by @cosmobysarah_ on insta</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtzu62</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1dtzo8y</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>How do you all get pictures that actually look good??</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtzo8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1dtze8x</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Citrus</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtze8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1dtzafn</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I tip extra next time to add more tip from the most recent service I got? </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtzafn/can_i_tip_extra_next_time_to_add_more_tip_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1dtz9ic</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail artist did great with these! </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06pxubufr6ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1dtyohv</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Just watching the clouds drift by</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqs08orrm6ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1dtyc9x</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails for wide nail beds? </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtyc9x/press_on_nails_for_wide_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1dtxxo7</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Confused what I’m getting done at the salon</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtxxo7/confused_what_im_getting_done_at_the_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1dtxjxi</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Apex of my nails keep on breaking?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7s0yrrrd6ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1dtxj0y</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite chrome </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ufyyewkkd6ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1dtxgen</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Ocean Nails</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtxgen</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1dtx8fh</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Can I do gelx on these nails?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtx8fh</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1dtx6oh</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Which type of manicure should I choose if I want to grow my nails?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtx6oh/which_type_of_manicure_should_i_choose_if_i_want/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1dtx2ma</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Draw me a design!!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aswrlh7y96ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1dtx1oa</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Loving my magnetics</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtx1oa</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1dtwrv7</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Turmeric Root and Bone</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtwrv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1dtwqe3</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>How come,</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtwqe3/how_come/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1dtwp5o</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Love pedi day🖤</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sredmqx576ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1dtwo25</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Nail Appreciation Post</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8a3sr8mx66ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1dtwmg1</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i 🩷 press ons </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxyo9sdk66ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1dtw7ek</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>holiday nails!</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19jiltkd36ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1dtw16h</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Mani rec: affordable, on the thicker side?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtw16h/mani_rec_affordable_on_the_thicker_side/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1dtvy2u</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Champagne Pink Polygel set</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtvy2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1dtvvtu</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>So happy with my new winter nails 🌀❄️💙</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptl7409u06ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1dtvra5</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5ifd0jvz5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1dtueib</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Blank nail tips for wide nails?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtueib/blank_nail_tips_for_wide_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1dtvadh</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>nails i’ve done over the past ~year!</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtvadh</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1dtvjww</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Festival nails 🩷</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10fvzbwcy5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1dtv8rq</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Recap of my favorites 😍</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtv8rq</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1dtv2y9</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>little heart ❤️</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtv2y9</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1dtv1uv</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Late Night Belle</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynvl2g3gu5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1dtv1lm</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>❤️🤍🩵 Ready for the 4th of July ✨ Painted Polish Red, White, &amp; Brew and Party Like A Patriot 2.0 ✨</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtv1lm</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1dtuwji</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>My nail tech is just 🔥</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixxi19lit5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1dtuuge</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Did my nails for my birthday</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtuuge</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1dtu7zo</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>HELP! My acrylic is coming off my nail, what do i do?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njzrs84ho5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1dtub62</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>My first time trying nail ornaments!</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/93t9trh3p5ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1dtu0zf</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Fourth of July nuls</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtu0zf</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1dtu06g</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>My Barbie Era 🎀</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by87kintm5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1dts55k</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Why do nail salons only apply tips with acrylic and not gel?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dts55k/why_do_nail_salons_only_apply_tips_with_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1dte3pe</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Where can I get a 100 pack of only small size nails?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dte3pe/where_can_i_get_a_100_pack_of_only_small_size/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1dtbf1i</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Can you buy Gel-X tips in certain sizes only?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtbf1i/can_you_buy_gelx_tips_in_certain_sizes_only/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1dtszqt</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Going to a wedding</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3quccg2bf5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1dtswwb</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Can you believe these are press on?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtswwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1dtrtkr</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Tips on limping this dip set along another week?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xs1fqnbq65ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1dtrohs</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Babyboomer with nail art, guess which one is an extension 🧐</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtrohs</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1dtrjmn</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Palm trees set</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtrjmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1dtc72x</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>WANT ADVICE (absolute beginner)</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtc72x</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1dtaj3z</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>nail inspo for these outfit colours? my hair is blue if that helps at all and ive no clue what shoes im wearing yet lol its fir my aunts wedding!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhyve30jj0ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1dtcosp</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">broke my nail how soon can i get them done? </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dtcosp/broke_my_nail_how_soon_can_i_get_them_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1dtr3kj</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>First time press on design?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtr3kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1dtj3xl</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Pulled an all nighter doing my nails, how do you like them?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtj3xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1dtr246</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Cute lil bows 🎀</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfwegku215ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1du7n4e</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Queen’s Crown Press-Ons</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du7n4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1du7mj8</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reminds me of 3D glasses </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lh5skk5qz8ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1du7hf0</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why does only cheap Claire’s nail polish work for me? </t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1du7hf0/why_does_only_cheap_claires_nail_polish_work_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1du6feg</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>What's an indie v. boutique v. drugstore? I am confused and this doesn't seem like a basic explanation</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1du6feg/whats_an_indie_v_boutique_v_drugstore_i_am/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1du63rk</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Summer chrome slime 🐸</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ieux49pi8ad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1du5ygz</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Swatch request: Dew polish Barbie Dreams</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du5ygz</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1du5ce3</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>So so short but dare I say they slay?</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du5ce3</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1du588w</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>June manis!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du588w</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1du54qi</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Holo taco top coat top coat with thinner or cirque top coat?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1du54qi/holo_taco_top_coat_top_coat_with_thinner_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1du5360</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Is Lights Lacquer worth it?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1du5360/is_lights_lacquer_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1du514b</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Golden Smog</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eveldhgg78ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1du511q</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>How on earth do I achieve this look</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apr5whek78ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1du3c75</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Happy 4th!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lkj82adr7ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1du2zvn</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Best dupe for sparkly sky blue salon polish?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4h7zf48o7ad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1du2sag</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Super Late but… My Pride Mani!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du2sag</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1du2idq</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Phoenix - Psionic (PPU June 2024) is phenomenal</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du2idq</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1du22ol</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fourth of July Mani </t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c6uorgrf7ad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1du1t1u</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Finally!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du1t1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1du1ihz</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Kathleen &amp; Co. - Cornflower</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h17ox76sa7ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1du13nj</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>much fussing</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du13nj</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1du0nvv</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Let's talk peel off base coat</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1du0nvv/lets_talk_peel_off_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1du0n0e</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>My sister. I want one of these</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uw5ig5uo27ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1du05ht</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Wicked Potion</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du05ht</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1dtyybp</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Recommendations for a dehydrator/primer (2 in 1? either/or?) for regular polish</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dtyybp/recommendations_for_a_dehydratorprimer_2_in_1/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1dtyv9v</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Had to get video in the sun. Sound on to hear my toddler's cute little "mom's"</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p39kavt9o6ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1dtyn3m</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Just watching the clouds drift by</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jze52lrgm6ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1dty5pr</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Subdolous by LynBDesigns -surprise thermal</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dty5pr</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1dty0ns</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Pistachio with pink/orange shimmer?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s40wv21fh6ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1dtx9d5</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Been trying everywhere to find this shade of electric blue in nail polish! Any suggestions?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ercapivfb6ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1dtx3qc</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>What I wore in June</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtx3qc</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1dtwyxz</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t xml:space="preserve">An Apology with a Little Gumption </t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtwyxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1dtwx6c</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>4th of July set I did last night!</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgp2b7yv86ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1dtwqmv</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>I am in love with ILNP</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dtwqmv/i_am_in_love_with_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1dtw9b0</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Help/Advice anything needed</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dtw9b0/helpadvice_anything_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1dtw8va</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Vintage dura-gloss® nail polish in “Century Red” from the ‘60’s</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtw8va</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1dtw6or</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Ok am I crazy or has LA Colors kinda stepped up their game?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtw6or</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1dtw4cm</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made a collage of all my manis to date for my IRL cake day! </t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcapiz9p26ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1dtv82c</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice to keep nails looking good despite chlorine exposure </t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dtv82c/advice_to_keep_nails_looking_good_despite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1dtuzu0</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>❤️🤍🩵 Ready for the 4th of July ✨ Painted Polish Red, White, &amp; Brew and Party Like A Patriot 2.0 ✨</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtuzu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1dtu5fz</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>🇺🇸</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3md2q02xn5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1dtu0vf</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Lurid lacquer burdock and buckthorn</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtu0vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1dttmv2</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Holo Taco Hot-Wire Pink</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dttmv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1dttltk</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Independence Day Picnic</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7l0xrcouj5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1dtt0is</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Poolside Gingham</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qf32g8bef5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1dtszp9</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Summery green french tips</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euggacqaf5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1dtskwk</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just got my PPU order in and oh my gosh I think I found my favorite polish ever </t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9y973lo9c5ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1dtsd88</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>4th of July Ready!</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtsd88</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1dtrqwc</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kypw3j565ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1dtrpb9</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Lime green summer</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtrpb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1dtresr</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Jellies that don't shrink?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dtresr/jellies_that_dont_shrink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1dtr7vw</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Heart of Sass - Sally Hansen Xtreme Wear. Feeling like I need to go back to Barbie Summer 2023. </t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtr7vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1dtr3yz</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Is MoonCat worth it?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dtr3yz/is_mooncat_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1dtr28a</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>I know we’re all focused on PPU rewind, but a quick mani from June</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7omflon215ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1dtqlw6</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Pinker than pink 🌷</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/pinker-than-pink-Imzpy0P</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1dtpcib</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Edm</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtpcib</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1dtosoy</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish High Quality Nudis (PPU Feb 2024)</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npodh0fjk4ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1dtonuw</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Lilac 💜</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n65uupljj4ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1dtoluz</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Black Cherry Berry 💋♠️</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypgbdw34j4ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1dto938</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Back into painting my nails after over a decade hiatus</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg3685vfg4ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1dtnaxa</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>My new favorite thing - first time trying Lyn B &amp; Deborah Lippmann</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtnaxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1dtm8ta</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Taste the rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtm8ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1dtm4ub</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swatch request 💜💚 PPU Whatcha Nightshade </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjm5kpc104ad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1dtln1g</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>[looking for recomendations] What are your favorite ballet core inspired nail polishes?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dtln1g/looking_for_recomendations_what_are_your_favorite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1dtlipd</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>I compared over 25 PPU rewind polishes on my IG</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtlipd</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1dtlgyw</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>First time trying a French manicure and i did it on myself! I’ll say I’m very happy with how they came out except for my pinky which i messed up. Any tips to improve in the future?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtlgyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1dtjuzn</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shade match question </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9ju0guqf3ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1dtj52a</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>I hate my job</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtj52a</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1dtivop</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Mooncat Field of elysium on natural nails</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtivop</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1dtgm7c</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>America, F*CK YEAH !</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2kkre2jd2ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1dtgm2b</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KBShimmer VS OPI strengthener </t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dtgm2b/kbshimmer_vs_opi_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1du5tx4</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like pink? </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axrlwegrf8ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1du5hau</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>🩷</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qn397kc2c8ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1du4jh8</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>I CAN’T HEAR YOUUUUUU! 🍍</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du4jh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1du3d7u</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>A detailed video on making nail art gel</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xyc9iwokr7ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1du2d05</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>mocha beach vibes ♡✿</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du2d05</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1du15y9</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Update IV added Bob to the set! I'm debating doing a 3d cut up credit card for his nail that Louise made him 🥴🤣 if I had space I'd have the burger of the day on a board 😭</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ukkd112o77ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1du15hg</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Update IV added Bob to the set! I'm debating doing a 3d cut up credit card for his nail that Louise made him 🥴🤣 if I had space I'd have the burger of the day on a board 😭</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bs6b1svj77ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1dtzdo5</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>My take on the cherry trend</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtzdo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1dtz38c</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>without a doubt an attractive and elegant design</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/48zylrpdp6ad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1dty2lt</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Summer nail art</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dty2lt</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1dtxob2</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>FROM ANOTHER PLANET 🌎 WHAT DO YOU THINK?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jfqe4lpe6ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1dtw2mx</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>What can I do to get a better result?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtw2mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1dttycx</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>I keep running out of nails</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dttycx/i_keep_running_out_of_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1dtt787</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I loved this design, what do you think?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzc18icvg5ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1dtri1y</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Palm trees set</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtri1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1dtqxhk</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>What’s your favorite way to plan out a mani?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dtqxhk/whats_your_favorite_way_to_plan_out_a_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1dtpz6n</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Fourth of July Nails (swipe for inspo pic) ❤️🤍🩵</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtpz6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1dto1cf</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Cheapest supplies for beginner</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dto1cf/cheapest_supplies_for_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1dtluwn</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Loving my unicorn nails / russian manicure so much! 🦄</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtluwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1dtky7i</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Nail art figurines that belong to girls themselves.</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dtky7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1dtkw0e</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brat when I'm bumping that </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ph950ohhp3ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1dtjrze</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>nail</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hk585uwe3ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1dtieyc</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Skull nails</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i95ju3t403ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jul  4 08:09:16 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_07.xlsx
+++ b/data/2024_07_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C684"/>
+  <dimension ref="A1:C873"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12062,6 +12062,3219 @@
         </is>
       </c>
     </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1dv0wp4</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>can i remove AND keep acrylic set?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dv0wp4/can_i_remove_and_keep_acrylic_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1dv0nn6</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Essie gel couture Bling it on short nails</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7l4m6lpagad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1dv045w</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Bridal nails for my big fat Indian wedding!🎀</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9kd4ewl4gad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1dv020q</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Strawberry 🍓</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aad2v5ly3gad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1duzexb</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>nails for my florida trip coming up!!!</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duzexb</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1duzbdg</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Loved this set. I’m still learning. This was all by hand and first time doing matte. Now to decide on what to do next 🤔</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b58iqdyovfad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1duyzuk</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Is this normal</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duyzuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1duyn8p</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>I've been doing my own nails for years, finally having fun with gel</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duyn8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1duyl71</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little pastel tie dye action </t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41vflkcxnfad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1duyjui</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>A few of my favourite nails I’ve done over the past year.</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duyjui</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1duyh6l</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Where My Press On Girlies? Kiss Is Having A Sale!!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>http://rwrd.io/bodnflz?s</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1duyeyq</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Me struggling how to pose to show off my nails</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duyeyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1duy51v</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>🤍🤍</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxa09i41jfad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1duxzd6</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Did my manicurist not paint low enough on my nail bed?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duxzd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1duxihw</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Marble &amp; Hello Kitty nails 💖✨</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duxihw</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1duxeqi</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>First time ever doing fruit nails!</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duxeqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1dux8l9</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>4th of July nails I did</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dux8l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1duwv4p</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Check out my beautiful man nails </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9cac06c6fad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1duwjwr</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>My summer nails</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrkqjjfe3fad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1duwiaw</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These could possibly be my favourite nails I’ve done </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duwiaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1duwg3e</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Strawberries 🍓</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m7mx4kc2fad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1dusgt3</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Not sure what to do about my next set? Any suggestions?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dusgt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1duw44k</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Old Rose</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7hxe4m5zead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1duw3vv</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>this ombré glitter is giving me LIFE 😻</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ea2d0jk3zead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1duvu66</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t xml:space="preserve">POV you do your own nails </t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duvu66</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1duvn8x</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Added a lil bit of shine</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4ke86vpuead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1duvfmn</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Obesessed w this set😍</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scfgluersead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1duva2l</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Looking for some summer nail color suggestions for my next manicure. Any ideas?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v1vt535read1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1duv487</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets the last year</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duv487</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1duuq2r</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Do these make my hands look better?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duuq2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1duujfp</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Cute galaxy nails ✨️🌌🌠🌛🪐</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duujfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1duuchz</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Before and after 😍</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duuchz</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1duu6ke</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>I’m in love I’m in love and I don’t care who knows it!!!!!</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jontyx82head1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1dutzkd</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Fourth of July nails</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mxdx83h7fead1</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1dutp4o</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freedom day nails! </t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dutp4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1dutlc4</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>{PR}Sassy Sauce | Tropical Heatwave</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dutlc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1dutbgs</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>some nail sets I’ve had</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dutbgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1dut29o</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>My July 4th nails!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufnm6z907ead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1dusxdr</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>First ever time getting acrylic nails, what do y’all think? Should I go back?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dusxdr</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1dusrgp</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>over a month retention!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dusrgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1dusnm7</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dusnm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1dus7po</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Gel X nails</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vtntbtnzdad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1dus4db</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>🧨🧨</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dus4db</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1dus1bp</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>New to nails, can i apply white acrylic over clear acrylic for my infills ?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dus1bp/new_to_nails_can_i_apply_white_acrylic_over_clear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1durvdp</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Pretty in pink 💕</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1durvdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1duruqb</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Around 5th time doing gel, tips for better brush work?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duruqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1durplz</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Selling Press-ons</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1durplz/selling_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1dur97m</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>🩵🌸</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dur97m</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1dur01u</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>SHARK ATTACK!</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dur01u</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1duqwyx</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>New nails for Florida 🏝️</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgzknhoyodad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1duqlev</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>builder gel tips?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duqlev</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1dulx3f</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If my filing of nails is unfortunately making my nails sharper (the filing makes them more uniform, but unfortunately the whole nail is getting sharper), what mistake am I likely making or what can I change? </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dulx3f/if_my_filing_of_nails_is_unfortunately_making_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1dudq1i</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Would I be able to put gel x on my nails?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75hlr908xaad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1dueyjq</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Press on nail art</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wr143mwg7bad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1dugar4</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Gel after 1 day</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jy5kgdbphbad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1du4smp</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Fresh set 💅 purple love💜</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zlmaaj858ad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1du51xb</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Inspired to post by oatmilksavesall</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1du51xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1duayyp</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Question about ordering press ons</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwo9kyvm5aad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1dud2xy</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Look at my purty nails.</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dud2xy</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1dud3u6</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>What I asked for vs what I got!</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dud3u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1duq5kx</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Marble press on collection</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duq5kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1dupz01</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>What do you think of the funky design?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dupz01</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1dupxg7</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Tried the butterfly trend for the first time. My husband convinced me post my work here.</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2ojcwsahdad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1duh8im</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>4th ever set!!!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duh8im</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1duhaki</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Wanna do my nails for the first time in my late 20s - help!</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1duhaki/wanna_do_my_nails_for_the_first_time_in_my_late/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1duiac8</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Significant curve on pointer fingers making it hard to keep press ons to stay - help?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duiac8</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1duo58r</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Dark blue and glitter gold nails, inspired by the night sky and stars 🌃</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duo58r</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1dup160</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>First time getting long nails, how did the tech do?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dup160</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1duoxow</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Summer vibe!🌼</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84c37u5t9dad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1duov28</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Fill with hard gel</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6mu0ja99dad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1duonym</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>What shape looks best on me?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duonym</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1duogi5</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>I feel like Sailor Jupiter</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duogi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1duockw</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>thought i make them this colour, dont know if im happy with it</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3p2nj24d5dad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1duo9hz</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>4th of July nails 🎆</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34469fkr4dad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1duo9dg</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing red </t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duo9dg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1duo57l</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqh8y1fu3dad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1dunw46</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Made myself some cute nails!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dunw46</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1dunuc2</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Total Black</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocw2sopl1dad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1duntx5</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>A nice plain white. Simple but pretty!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duntx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1duncnu</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>My set for Butterfly Wonderland in AZ</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duncnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1dun6oq</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with my new big French </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dun6oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1dun4jl</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rainbow custom order </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whxsuk20wcad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1dun1ss</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Minimalist Magic ✨🌷</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npv20xjkvcad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1dumdi5</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Love a simple french tip☺️</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ri1n49piqcad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1dulz8a</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Toy Story!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dulz8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1dulw5k</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>My new obsession is the BTArt box nail kit! DIY and lasts 3 weeks!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qw747jhxmcad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1dulgx6</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Soft gel tips </t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dulgx6/soft_gel_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1dul9pi</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Is this normal nail growth for 1.5 weeks?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kefvsu7icad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1dul207</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Is there a way to like ensure slope?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5bokq2ogcad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1duktlg</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Put them on, and I never wanna take them off 😍</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duktlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1duki7l</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Manucurist nail oils + masks</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1duki7l/manucurist_nail_oils_masks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1duk1x3</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>In memory of my bestfriend that passed at 27 last year. Nail credits to @nailsbykell</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duk1x3</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1dujtid</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>pov: i'm farm vet surgeon</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvrrq00j7cad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1dujt27</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>new pressies by me 🐚🪸🌊</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dujt27</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1dujp9n</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>First attempt at gel by myself</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dujp9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1duje15</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>summer french pedicure</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jexks45h4cad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1duj96t</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Monstera Nails</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duj96t</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1duj7c2</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Mixed Berries</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au052ko23cad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1duirfi</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Didn’t mean to match but loving that it does</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yr93fvrzbad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1duipw3</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Cute last minute 4th of July nails I did 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duipw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1dv0kzx</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Independence day!</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93ddy9xw9gad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1dv08qp</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Need some help</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dv08qp/need_some_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1dv03ue</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>How to stop snaps?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywi57f9j4gad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1duz39p</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Should the Polish be closer to my cuticles? Or am I just being picky?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duz39p</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1duyv6u</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>do you guys fly thru bottles of polish?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1duyv6u/do_you_guys_fly_thru_bottles_of_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1duxuym</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Mooncat sent me to urgent care 🥲</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1duxuym/mooncat_sent_me_to_urgent_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1duxm9m</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Excuse my mess, I haven’t cleaned them up yet because I can’t tell if I hate the color on me</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duxm9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1duvkkn</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Ready for spooky season 👻</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duvkkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1duvhpp</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Forbidden Pop Tart Frosting</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duvhpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1duveqc</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>“I am the Confusion” (06/24 PPU)</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duveqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1dunbkj</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>🌙🐈‍⬛ Mercury's Tears</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0hjg7omxcad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1dulryp</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Help with Polish Pick Up July 2024 PPU Rewind List</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dulryp/help_with_polish_pick_up_july_2024_ppu_rewind_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1duuyan</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>How do you know what nail shape is most flattering for your fingers?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1duuyan/how_do_you_know_what_nail_shape_is_most/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1duu68d</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>What are your favorite brands / colors in this color palette? Just did my color analysis &amp; wanna treat myself 💅🏽</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnp7az4zgead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1duu2t8</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>4th of July themed shopping my stash</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fscclv4gead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1dutsp1</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Have you put on cuticle oil today?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dutsp1/have_you_put_on_cuticle_oil_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1dutoqn</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>{PR}Sassy Sauce | Tropical Heatwave</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1xyhmqfgcead1</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1dutne0</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>starry eyed ✨</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lk8o1io5cead1</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1dutije</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Getting into polish and my new ILNP shades were perfect for this week!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cs8y6cyaead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1dutc7k</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Ready for the 4th</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dutc7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1duscn9</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>3+Weeks SH Miracle Gel</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duscn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1dus9om</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>3+Weeks SH Miracle Gel</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dus9om/3weeks_sh_miracle_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1duryt9</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>I found the perfect interview polish</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duryt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1durxs0</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">On Wednesdays we wear red </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89sxmsyxwdad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1dur89r</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>My bf said to do dragon egg nails… I think I did okay XD</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dur89r</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1duqvhr</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Did I just do my nails four days ago? Yes. Am I probably taking it all off and redoing them AGAIN tmo because I have new Mooncats coming? Also yes 💅🏽😌</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duqvhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1duqdbi</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>I guess I know what I like?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afjuyp7rkdad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1duq9pe</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Trying to create a Latte Cloud dupe</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duq9pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1duq997</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Essie A-List</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wr2j5hkvjdad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1duq1bi</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This polish matched perfectly the echinacea in the background </t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybz6b4t5idad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1dupnm4</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Does anyone know of a close color match to OPI’s Massachusetts Mulberry?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5p8l078fdad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1dupb0i</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you take photos of nail polish that look nice? </t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dupb0i/how_do_you_take_photos_of_nail_polish_that_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1duoieg</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t xml:space="preserve">An oldie but a goodie </t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duoieg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1duo60h</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Someone tell me I don’t need it 😫</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yoya3jk04dad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1duo4z1</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>4th of July jelly nails</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekcnfd9n3dad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1duo18o</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best white polish? </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1duo18o/best_white_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1dun21o</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>I gotta try layering ILNP polishes over each other more often 😍</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dun21o</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1dums5g</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>I think this is the best job I’ve done painting my own nails!</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tjpdomhtcad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1dulmrp</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>How??</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dulmrp/how/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1dulam5</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>How gorgeous is Cadillacquer's "Neptune"!?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dulam5</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1dul8ye</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Give me BRIGHT</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dul8ye</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1dul01k</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Lush by PFD</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dul01k</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1duknmm</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>cannot believe i slept on her for so long 😭</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/voc3bccsdcad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1duk9w5</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Can french tips look good on uneven nail lengths?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1duk9w5/can_french_tips_look_good_on_uneven_nail_lengths/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1duk7tg</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fav Removers? </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1duk7tg/fav_removers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1duk64d</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love 😻 </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/flh3n5u3acad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1dujl1q</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Mooncat - Moonicorn 😻</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xot31cru5cad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1duiga8</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>help with using the glisten and glow top coat/user error?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1duiga8/help_with_using_the_glisten_and_glow_top_coatuser/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1duid3r</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💖🩵🌵Yeehaw🌵🧡💖 </t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duid3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1dui4pu</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>So mesmerizing!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lfbh6hh3vbad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1dui38o</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Best 1-coat blurring base</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dui38o/best_1coat_blurring_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1duhuj8</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Fourth of July skittle</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzzafv11tbad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1duhu2y</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Zoya 4th of July sale: 10 polishes for $25 select colors, ends 7/7</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl9u4spxsbad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1duhbkf</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Dragon fruit was the Inspo 🩷</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3dq8sx4pbad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1duh7ju</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Solar Power 😍</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duh7ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1dug6yw</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>My nail beds seem to lose all of their color when I clear coat them :(</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drsiphfxgbad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1dufrfk</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lumen Moon Prism Power </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/311rziqndbad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1dufkx2</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>in love with these juicy jellies 🍑🍓😋</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpe68lc8cbad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1duf9m3</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>🧨🧨</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duf9m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1duf9dz</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Essie like it loud vs licorice</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1duf9dz/essie_like_it_loud_vs_licorice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1dueztl</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>mooncat “the diabolical mojo jo-jo”</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0uwigtxq7bad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1duea2c</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make my nails look healthier? </t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duea2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1due5nu</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>OPI formulas are -not great- but once I added thinner...</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/518g71hn0bad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1dudz5h</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Porcelain Nail Art</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dudz5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1duduw3</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Wow glass nail files are amazing</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1duduw3/wow_glass_nail_files_are_amazing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1duclwt</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Grungy 4th of July?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duclwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1ducbpx</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“House of Hades” from Mooncat + playing with macro </t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ducbpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1duc6hc</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Mainstream brands make bangers too</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yaf8zqduiaad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1dv1k3k</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>first gel french tips</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv1k3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1dv01hc</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>mermaid on natural nails</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv01hc</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1duzugx</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Aimed for marble, landed at y2k goth adjacent</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ntfe3jl1gad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1duy9nu</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>First time using blooming gel</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8cvp97gkfad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1duxbjd</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Ocean vibes</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duxbjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1duw1az</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Had to try this trend out</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wl7a41fyead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1duvvq0</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>I'm happy because the brush strokes came out</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/902blm1twead1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1dutkss</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>4th of July Ready!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dutkss</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1duqp2b</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Is this a stupid idea?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6mwhg1s8ndad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1dupzjx</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Marble press on collection</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dupzjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1dupo10</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Inspiration to love ❤️ 👄</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56gnnofbfdad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1duobcy</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>USA 4th of July Nails</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iu5nej665dad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1dunk6x</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Nail Techs, Is it bizarre if the client offers to bring supplies?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dunk6x/nail_techs_is_it_bizarre_if_the_client_offers_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1dumr9x</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Something different..</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dumr9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1dumnxp</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>When the press ons look like acrylic 🤌🏼</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dumnxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1dul02z</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Immersive Handmade Nail Art Creation</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s60frq58gcad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1dujz9w</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>In memory of my bestfriend that passed away at 27. Nail credit to @nailsbykell</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dujz9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1dujyjm</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>My designs</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dujyjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1duhrsj</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Independence Day nails 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duhrsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1dugvda</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>These were fun to do</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dugvda</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1dud47k</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>My first and second attempt with Blooming gel</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dud47k</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jul  5 08:09:08 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_07.xlsx
+++ b/data/2024_07_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C873"/>
+  <dimension ref="A1:C1056"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15275,6 +15275,3117 @@
         </is>
       </c>
     </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1dvrrns</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>First time doing French in years</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghu847dcenad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1dvqsuq</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>15$ nails</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zv4jf5z2nad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1dvqpm1</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Chrome+matte is so cuteee!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvqpm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1dvqgxv</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my nail tech </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p95maw6zmad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1dvq9xa</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Not mine! But these are just soo damn cool</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ie5i70exwmad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1dvnbqd</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Nail shape?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvnbqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1dvoagr</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>literally obsessed with these!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvoagr</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1dvp67p</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which nail polish color should I do for my next manicure </t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvp67p/which_nail_polish_color_should_i_do_for_my_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1dvq65r</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Berry tones🍓</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/roc01sunvmad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1dvq5lp</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>First try at gel nail art. Just applying it is harder than I thought! Advice?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8a4uzfhhvmad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1dvpwa4</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>I need advice</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvpwa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1dvpvln</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Love 💕</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6j8iyohsmad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1dvpqv3</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand painted eyeballs done by me! </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx8hc2ozqmad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1dvoz8r</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>What do you consider a good tip?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvoz8r/what_do_you_consider_a_good_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1dvoutc</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gotta moisturize my cutes, hate the oil spill </t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvoutc/gotta_moisturize_my_cutes_hate_the_oil_spill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1dvolw5</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Suggestion please</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvolw5/suggestion_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1dvogi8</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Need tips for frenchies</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uj0m26rxcmad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1dvoeyh</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Obsessed 💙🦋🧢🔹🌀</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvoeyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1dvo7c5</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>My strawberry 🍓 submission</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkcn06faamad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1dvnhbx</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Any tips?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvnhbx</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1dvn8pm</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>How long do you usually wait to get a fill in?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvn8pm/how_long_do_you_usually_wait_to_get_a_fill_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1dvn2pf</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Appreciation post for my nail tech </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvn2pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1dvm8wo</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>I love my nail tech</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvm8wo</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1dvkhrn</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Suggestions?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvkhrn/suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1dvlzt1</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hard gel, dimensional set in shimmery nude with luminescence </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvlzt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1dvlbj8</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4th of July nails - first time doing nail art </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvlbj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1dvl3qk</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvl3qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1dvl2m2</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Hand sculpted/painted color changing beer nails</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5svn16t7dlad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1dvkvo6</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Olive green cat eye nails!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jvwa2d3eclad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1dvkum0</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Growing out nails - Can I get clear builder gel alone with no polish? More in post </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvkum0/growing_out_nails_can_i_get_clear_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1dvkuib</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Advice for gel nails.</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvkuib/advice_for_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1dvktbl</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Obsessed with making press ons for all of my friends 💕💛🧡</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7xa4t9sblad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1dvkim7</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">❤️❤️❤️I loved them </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imae2xuw8lad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1dvk772</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel like me again. </t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvk772</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1dvjqtm</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>My 4th of July nails 🍒</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6sy65lt1lad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1dvj470</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>“Black with Rainbow” nails as requested by my 4yo son.</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvj470</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1dvjxdx</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>My nail lady did it again!!</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvjxdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1dvjvk6</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Feeling the Heat</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvjvk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1dvjnql</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>my first try at some nail art!</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvjnql</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1dvjn8k</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Flower Power!</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvjn8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1dvj9wu</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4th of July nails I did on my SIL! (I’m not licensed I just do them for free) </t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvj9wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1dvj5px</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Monarch 👸🏾🧡</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9e4rfmjwkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1dvj3p6</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Need help/Advice for a new diy person</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvj3p6/need_helpadvice_for_a_new_diy_person/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1dvizmo</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Reg. Polish Milk Bath Attempt w/ Cirque Colors Kismet</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvizmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1dvi10n</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>help me decide which nail shape and length suits me best?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvi10n</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1dvifaz</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Jojoba and vitamin e oil mix</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvifaz/jojoba_and_vitamin_e_oil_mix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1dvg8m2</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Tried a Beach Inspired Look</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrsll80f8kad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1dviu9g</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Pretty pink press-ons</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dviu9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1dviogb</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>How can I improve my nails?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv2egcydskad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1dviign</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>I found a new nail girl and I’m obsessedddddd</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dviign</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1dvigi0</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>So glossy 😍</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvigi0</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1dvig1l</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Did I waste my money?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35ftp9ueqkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1dvieeo</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Vacation set 🏝️🧡</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdv55hs0qkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1dviafc</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Matte green</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ziffjma2pkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1dvhpqi</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Girly vibes 💕💗</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91zlt899kkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1dvh96n</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Happy 4th of July! 🤩</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvh96n</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1dvh618</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Nails for Olivia Rodrigo concert🤩</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozn3anxtfkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1dvh2a9</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>I don't usually use glitter but I really liked it! what do you think 🫶🏻🥹💅🏻</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kq6kjg0fkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1dvgtml</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>First time acrylics!</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvgtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1dvgphm</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4w9qo037ckad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1dvgkz6</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Powerpuff girl 💚</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/790fepo6bkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1dvg7kv</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Shoutout to my nail tech, I am loving this watercolor technique!</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1j5tly28kad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1dvg4bw</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>3rd times a charm?🧜🏾‍♀️🩵</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvg4bw</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1dvg0ly</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>New claws</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01fqgcdn6kad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1dvfxy1</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gave my favorite client a free set </t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9n7ejm16kad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1dvfs6r</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Firework nails</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zim8dhat4kad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1dvfrmg</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Hi! New to nails etc, and I have some Qs before I get mine done for the first time!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvfrmg/hi_new_to_nails_etc_and_i_have_some_qs_before_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1dvfoy5</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Anyone ever bought from premier nail supply?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kbkrsj34kad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1dvfohc</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Now I can give people the flaminger!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/724ysh204kad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1dvffqf</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>i used to bite my nails as a kid , is it my fault [some of] my Acrylic nails come out like this?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvffqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1dveuye</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>I love my nail technician</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3a6tz2jfxjad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1dvewm5</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>At home mani</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u08mrtgtxjad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1dves1p</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Hand painted gel nails 👁️💚</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dves1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1dverex</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>I feel like I don’t suit coloured nails. Can you advise me on colours?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dverex/i_feel_like_i_dont_suit_coloured_nails_can_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1dveqa7</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>First try with design brushes!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s08b366ewjad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1dvepu4</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Chrome pink nails 🩷</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1spcqeawjad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1dvem2v</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>first acrylics done by me</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvem2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1dvei7q</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Patriotic nails</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvei7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1dvegy2</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Color change/glow in the dark 4th of July ❤️🤍💙</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bbke61w8ujad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1dveeof</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>4th of july set🎉🎉🤍</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dveeof</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1dve14k</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just here to show these off </t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dve14k</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1dvdrxt</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>I pushed backed my PNF</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvdrxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1dvdg3l</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>My 4th of July nails! Still getting the hang of gelly tips</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qkq99fcmjad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1dvdcqz</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>new nails 🖤</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvdcqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1dvdcdl</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I being overly critical? I went back to the salon and had my thumb acrylics shortened but now I feel like it’s too thick (on both hands) i’m debating going to another salon to have both thumbs totally redone cause i kinda hate it  </t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q12xnjsgljad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1dvdby6</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>2nd time trying poly gel :) small cat approved</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvdby6</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1dvdarr</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>My strawberry nails!</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqz5gufaljad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1dvcl5x</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Temperature gel.❤️</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvcl5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1dvcj2d</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Holaaa from the Canary Islands!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvcj2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1duw7q8</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Please advise me on the best thing to do</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duw7q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1dvawst</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Did I pay too much? ($90)</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvawst</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1dv9xbe</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Summer nails :)</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv9xbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1dv8d6v</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Can you have healthy nails while using press ons with glue or sticky tabs?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dv8d6v/can_you_have_healthy_nails_while_using_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1dv7vzv</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Tried to go for a chrome, iridescent space inspired look, what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv7vzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1dv7opm</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Pink velvet 🌸</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv7opm</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1dv5a2e</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Considering a switch to acrylics but scared!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dv5a2e/considering_a_switch_to_acrylics_but_scared/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1dv4wm0</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for some inspo for a fall acrylic set! My dress is green! </t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dv4wm0/looking_for_some_inspo_for_a_fall_acrylic_set_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1duxktu</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>My Birthday Set For Gemini Season This Year :)</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1duxktu</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1dvbz26</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Friendly reminder to tuck your bangs 🥲</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhowqgc2bjad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1dvbqg3</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Types of extensions?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvbqg3/types_of_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1dvpuqh</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethereal Lacquer Lorraine </t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvpuqh/ethereal_lacquer_lorraine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1dvpd2h</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>ISO gray/blue polish with pink and/or gold and/or green irregular flakies</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvpd2h/iso_grayblue_polish_with_pink_andor_gold_andor/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1dvp7nk</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which nail polish color should I do for my next manicure? </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvp7nk/which_nail_polish_color_should_i_do_for_my_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1dvo78g</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Also in my villain era ^-^</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4qebhk4amad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1dvo42b</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Night Owl 🦉</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52lh9o6b9mad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1dvo3c6</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seeking to dupe Lemmings Lacquer Euphoric Embers </t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvo3c6/seeking_to_dupe_lemmings_lacquer_euphoric_embers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1dvnfee</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>A pleasant suprise</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/4-7-2024-smZiSeX</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1dvn7p9</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Nails peeling after less than a day</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hmcu5820mad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1dvly0s</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>What’s Up With Color Club’s Pricing?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uktklvmzmlad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1dvlvtz</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Neon pink 🦩☀️</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvlvtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1dvltz7</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Oh say can you see</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/5lUNbjJ.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1dvl28p</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>I was craving a jelly(ish) sammy 🍞🥪🧚🏼</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrwm5v55elad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1dvkffj</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>First try at French tips! I have shakyyyy handssss 🥲</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvkffj</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1dvk7am</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>“Don’t Put Me Down for Mummification” from LynB Designs. This one’s a real shifter!</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvk7am</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1dvk403</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>A new idea for myself, and a little rough. Next time will look even better!! 🖤💖</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jlr3u4u25lad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1dvjzeq</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>First time with flakies, how did I do?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvjzeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1dvjung</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Feeling the Heat</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvjung</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1dvjtqa</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Day before’s nails!</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nxa0oui2lad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1dvjb2j</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>“Twilight Shimmer” over black 🤤</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvjb2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1dvj614</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>ISO: Neon coral (leaning orange) crème nail polish!!</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvj614/iso_neon_coral_leaning_orange_crème_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1dvj4zo</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Emily de Molly- pinkie swear</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvj4zo/emily_de_molly_pinkie_swear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1dviscq</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Shiny Happy Pea-ple 🫛</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dviscq</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1dvip88</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>did my nails for the 4th!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvip88/did_my_nails_for_the_4th/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1dvip0u</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>We love you Kevin Bacon</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vkqat3jskad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1dvikk8</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>BKL - Through Love, All is Possible</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvikk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1dvien2</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Happy 4th of July!!!!!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbliwaj2qkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1dvic3y</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decided to swatch my entire collection. </t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fusadcogpkad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1dvi4sn</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Recommendations for best quick dry top coat in PPU</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvi4sn/recommendations_for_best_quick_dry_top_coat_in_ppu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1dvgnu9</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>how to remove skin stuck around the nail</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67vjntnubkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1dvhvkz</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Pest control is hard on the nails 🥲</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5234enellkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1dvh2yk</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Comparison between Mooncat’s Chemical X and Holo Taco’s Everything Taco</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2nkjd06fkad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1dvgwf0</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Lavender Sunset 🌅🌄</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvgwf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1dvgtxd</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>nails match my tamagotchi! ✨💫</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvgtxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1dvg7tz</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling summery </t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l14vg2x88kad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1dvfzt7</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is your reminder to BE NICE to other people </t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvfzt7/this_is_your_reminder_to_be_nice_to_other_people/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1dvfvok</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Brb, in my villain era</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4pag29l5kad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1dvfu8j</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Essie Mademoiselle</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tranahsa5kad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1dvfqdh</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Firework nails</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvfqdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1dvf2xh</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Does mooncats speed demon top coat have toluene in it?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvf2xh/does_mooncats_speed_demon_top_coat_have_toluene/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1dvetsk</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Strawbs for summer</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjh915l6xjad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1dve8yg</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Best ridge fillers?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dve8yg/best_ridge_fillers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1dvdyqa</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Experiment - Chrome tips </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3wiabadqjad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1dvdjav</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Smith &amp; Cult - Seek Me Out</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvdjav</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1dvd4zz</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reflective glitter is my new favorite thing :-) </t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvd4zz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1dvch1k</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Independence Day nails </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my17xg1wejad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1dvcfal</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">White Crellies? </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvcfal/white_crellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1dvc5qc</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I get this effect? Looks black but shifts to pink depending on the light. </t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ze6bpt7hcjad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1dvbz60</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Happy 4th🇺🇲🎇🎆🇺🇲</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vltdlx13bjad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1dvbx7o</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Essie pencil me in</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9nffm4oajad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1dvay1e</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Oh Popeye - Sweet and Sour Laquer</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6awqbnr43jad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1dvay11</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Mooncat Dupes (Since I dont trust their bottles)</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvay11/mooncat_dupes_since_i_dont_trust_their_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1dvae5u</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Pastel Daisies! &lt;3</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvae5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1dv9q3y</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>4th of July, SOAD style</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv9q3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1dv9127</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Londontown kur</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dv9127/londontown_kur/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1dv90qg</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Game over.</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iakzuq4coiad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1dv8p6p</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Garden of evil looking fly as hell</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ertkbzduliad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1dv8o6s</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>🌭 Ready for the BBQ 💥</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv8o6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1dv8mq8</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Advice on nail structure and shaping using forms</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv8mq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1dv89my</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Happy 4th of July!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw1717feiiad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1dv84s9</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>How many of you have been cut by or had furniture damaged by Mooncats polishes?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dv84s9/how_many_of_you_have_been_cut_by_or_had_furniture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1dv83vz</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>ethereal lorraine swatched on an opaque stick</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dv83vz/ethereal_lorraine_swatched_on_an_opaque_stick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1dv6knq</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>i can't stop looking at it</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv6knq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1dv6dbb</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>How can I avoid the nail drill at the nail salon? I’m so afraid but I love dip/gel overlay 😖</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dv6dbb/how_can_i_avoid_the_nail_drill_at_the_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1dv5t5g</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Atomic’s neons are so good</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv5t5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1dv57tn</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Fourth of July 🎆</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv57tn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1dv56pb</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>July 4th mani</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1qsbis9rhad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1dv4u00</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Clearly I have a type 😅 Possible Zoya 4th of July Sale purchase</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv4u00</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1dv4o0b</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>An abstract interpretation of July 4th ♥️</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wij22buylhad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1dv4loj</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>First attempt at nail art! Not perfect but I'm pretty pleased with the result. Happy independence day from rainy England. (Yes I see the irony.)</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dv4loj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1dv20ne</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>do people actually use thermal polish?</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dv20ne/do_people_actually_use_thermal_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1dvqx9g</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>A detailed video on making nail art gel</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hzh4wl1g4nad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1dvpilb</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>My first attempt at tortoiseshell nails 💕</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ueocgy6fomad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1dvn372</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Black almond red bottoms</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvn372</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1dvi77q</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>My first attempt at press ons!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd93k0raokad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1dvfimx</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>4th of July nail art</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uecsa0p2kad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1dvdw32</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>First time trying almond nails and obsessed. I’m a sl*t for coffin but wanted to try something different. @ferdoesnails on IG</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/530x5v6tpjad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1dvdqai</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>This is a mini drawing tutorial caton drawing of lucas duck ✨️💖 made by me. My instagram is @ab_nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w9b7nkwgojad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1dvdife</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Life's a beach, Babe</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvdife</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1dvcoea</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>✨Swirls &amp; stars ✨ (home mani with regular polish)</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvcoea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1dvapc4</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Really love my new nails</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvapc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1dv9acn</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>The Nails Bae Freestyle Set</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3gky04fqiad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1dv6efu</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Why is my color gel doing this?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crvzzdyu2iad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1dv48i4</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Took me 2 months and I'm still not happy</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scy16qwehhad1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jul  6 08:09:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_07.xlsx
+++ b/data/2024_07_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1056"/>
+  <dimension ref="A1:C1234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18386,6 +18386,3032 @@
         </is>
       </c>
     </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1dwkioj</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Nails master</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwkioj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1dwk03i</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to protect pedicure in tennis shoes? </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dwk03i/how_to_protect_pedicure_in_tennis_shoes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1dwjvs5</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Lovin the color❤️</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egc1wjh2muad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1dwjacu</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>One of my favs I’ve done</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwjacu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1dwh4ki</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>🩵</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwh4ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1dwh3lz</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with CIRQUE nail colored please </t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dwh3lz/help_with_cirque_nail_colored_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1dwg89j</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Would you pay $105 for these?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyag2f9yhtad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1dwfzwk</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>It’s giving r/nails sub</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfhfzl1lftad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1dwff0x</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Self taught with beetles gel</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwff0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1dwfboe</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>One of em popped off, but not to worry!!!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwfboe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1dweuv5</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Im trying to go natural can I get some help</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h83b5vuk4tad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1dweapi</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>I went a little longer than usual but I am obsessed! 💗</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dweapi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1dwdrgc</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>first time doing my nails (m)</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i5ifo53usad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1dwdmyu</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Salon French manicure full set</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnal7p8yssad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1dwdbuy</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>first gel x set ever - tips?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwdbuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1dwd4x1</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time yesterday! I am in love😁</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwd4x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1dwcmai</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Is it too early to give up?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8igolsmljsad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1dwc5c5</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Help me choose</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1mix6sjfsad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1dwbmci</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Pick n' Mix Nails</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwbmci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1dwbq2a</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Can I trim down gel nails myself?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dwbq2a/can_i_trim_down_gel_nails_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1dwbk7t</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did some flower toes today! </t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bhk7v9masad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1dwbhus</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what’s special about cuticle oil? </t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dwbhus/whats_special_about_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1dwbhpc</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cute lil frenchies I did the other day </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwbhpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1dw95br</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>I’ve had acrylics since October and I have fungus all over my nails…back to press ons.</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tumy81gcrrad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1dwb3qi</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Excuse the mismatched socks</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3a9ecyw6sad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1dwb2xn</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Swatch collection</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwb2xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1dwarw6</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Simple glitter ombre</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwcr63694sad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1dwapg3</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Pretty  💗</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmxedlpq3sad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1dwal20</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>I wanted a more orange colour but the salon was out, so I got this instead</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwal20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1dwadhs</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Difference between Gel X and Acrylics?</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dwadhs/difference_between_gel_x_and_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1dwabfv</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Nails by @toxicaclawz</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwabfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1dwa56f</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Acrylic Nail Removal @home</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dwa56f/acrylic_nail_removal_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1dw9vho</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Took me 3 hours but I love my dip glitter french manicure </t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8ms3oy5xrad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1dw9v2c</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>My niece has a horror theme birthday coming up so i did her nails for her!!!!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw9v2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1dw9bkv</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Just to make y’all laugh</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dw9bkv/just_to_make_yall_laugh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1dw91tg</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Can we admire her nails??</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f82c8fnkqrad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1dw8zk0</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Leopard nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw8zk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1dw8vcy</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Come on Barbie, let’s go party 🩷 🪩🥳</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2aauq3k2prad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1dw8eq8</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Rate my Simpsons nails</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw8eq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1dw8ddt</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glue </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dw8ddt/glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1dw89eo</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Press on life</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tuv3sk1ckrad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1dw7vwl</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>This is my right hand 😭</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw7vwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1dw7nvi</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>nail help!!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dw7nvi/nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1dw73y3</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Candy Moyo nail polish is so UNDERRATED!! Im in love with my nails🤩🤩.</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw73y3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1dw71tu</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>First at home manicure, thoughts?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmttra4varad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1dw6z6r</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>💧details💧</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8eppq6carad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1dw6u97</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Happy Birthday to me!!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw6u97</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1dw6t1n</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Why have manicurists started going so hard on the cuticles?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dw6t1n/why_have_manicurists_started_going_so_hard_on_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1dw6rjr</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">need assistance locating YSL No. 1 Rouge Pop Art, as it is no longer available. </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dw6rjr/need_assistance_locating_ysl_no_1_rouge_pop_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1dw6h6s</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>yum 🌞</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw6h6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1dw6f0d</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Mermaid nailz💧💧💧</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3aq28zy5rad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1dw68ut</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I use one of those electric, rotary "nail drills" or "nail files" to just simply file my nails down instead of clipping them? </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dw68ut/can_i_use_one_of_those_electric_rotary_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1dw5qlh</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Similar style </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw5qlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1dw5qsh</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Pretty in pink 💗</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8rekkzr0rad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1dw59xf</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UV Gel question </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dw59xf/uv_gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1dw56yx</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>What I got vs inspo pic from Pinterest</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw56yx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1dw563f</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>I love these</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lq3gujegwqad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1dw3j82</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>I haven’t done a multi colored nail in quite awhile, so when I saw this color inspo on Pinterest, I hopped on board. 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw3j82</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1dw320n</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>First time getting nails done Help? Credits to @itss_sandraaa on TikTok</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgsw89ddgqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1dw4xme</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>New Ring 💍</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvodqpwjuqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1dw4s66</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Chop chop</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw4s66</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1dw4r0r</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>$7 nails</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eapivg87tqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1dw4nbl</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>got my nails for 850 PHP (14 USD) 😸</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1n9abiffsqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1dw3pf3</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Pride Month may be over but I'm proud of who I am! My Nail artist is Amazing!!!</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw3pf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1dw3mm3</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💅 💜 Feeling pretty 🤩 What do you think? </t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l66sos8qkqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1dw3hl3</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Need help finding my nail unicorn</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dw3hl3/need_help_finding_my_nail_unicorn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1dw38lq</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Red glitter shorties</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw38lq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1dw38cy</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>What do you think ?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw38cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1dw2xod</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Bright Wildflowers 💐</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw2xod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1dw2x9x</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>First rave - had to make matching nails</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3yinv6cfqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1dw2ses</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>OBSESSED 😭🎀💅🏽💘</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqgzbu8aeqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1dvt5tk</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>I was feeling weird</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9vqypelvnad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1dw121m</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>X- Nails brand suggestions for basic prep work?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw121m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1dw0232</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Critique and tips ( Reddit keeps washing out my first picture) </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw0232</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1dw206u</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>mix and match 🍅🍅🍅🍅</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctf808gc8qad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1dw1z3l</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>I love this color</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw1z3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1dw1ego</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>I'm undecided between these two colors to do at the next appointment</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw1ego</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1dvzuni</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Purple sparkle</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24zlwn5krpad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1dvzduo</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>First time doing my own nails!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwbwqqnunpad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1dvz4tt</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>How can I stop flooding my sidewalls with gel? I can't work out why it happens and looks bad even though it seems even.</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvz4tt/how_can_i_stop_flooding_my_sidewalls_with_gel_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1dvz1hc</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Classic white ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lbxtcn1lpad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1dvyi1s</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>New to doing gel nails- how to improve!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f67cr6ykgpad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1dvxzij</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">just a lil nail art to match my fourth of july dress </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvxzij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1dvxowq</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Clear gel polish with a pink and gold aurora powder</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ifgwr0kr9pad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1dvxnog</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Natural: How long is too long for my natural nails?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvxnog/natural_how_long_is_too_long_for_my_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1dvxip9</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Which shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvxip9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1dvx446</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>How many fills untill a soak off?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dvx446/how_many_fills_untill_a_soak_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1dvx09c</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>gel nails I did for a friend!</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wrecgxzo3pad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1dvwjrm</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Got my nails done</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvwjrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1dvwcp3</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>🧿June🧿</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvwcp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1dvv5pt</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>cherry color will never go out of style</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khcep24jkoad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1dvv5f0</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>asked for ombre..</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kob2c6sekoad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1dvusd9</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Gutted, Ive only had them 1 week.</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvusd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1dvurom</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>im looooving my new set</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvurom</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1dvuc35</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Nail art for the Calgary stampede!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85neha6qaoad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1dvtv9q</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Home made nails, thoughts?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsje1csm4oad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1dvtj5f</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Homemade</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4c5a98gf0oad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1dvtd13</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Que os parecen?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3izru47ynad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1dvtbl7</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zx4aqfpxnad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1dvt63x</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Gel nail advice!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cooi3r2pvnad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1dwk70o</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>searching for a pink to white thermal!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwk70o/searching_for_a_pink_to_white_thermal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1dwk3zt</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Way to Get specific KBShimmer polishes in Canada?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwk3zt/way_to_get_specific_kbshimmer_polishes_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1dwjy8w</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>The perfect match</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgtv6slzmuad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1dwjs9m</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>I Scream Nails Badass Berry topped with ILNP Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwjs9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1dwi5pf</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>How do you cut your toenails?? Straight? Round?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwi5pf/how_do_you_cut_your_toenails_straight_round/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1dwh7zy</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Grumpy Bear</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwh7zy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1dwh4pc</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help with CIRQUE colours please </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwh4pc/need_help_with_cirque_colours_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1dwh498</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>I keep getting bubbles!!</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwh498/i_keep_getting_bubbles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1dwg52m</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>I am captivated by this one PLUS new nail shape</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i0jpdrzygtad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1dwfrgk</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>RaspberryMarmalade</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3tmufcp9dtad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1dweqe0</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Haul Part One</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5obg674e3tad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1dwdxwe</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Painting Nails While Sick</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwdxwe/painting_nails_while_sick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1dwdwb5</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>With all the Mooncat drama, does anyone have a dupe for “Getting Even”?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwdwb5/with_all_the_mooncat_drama_does_anyone_have_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1dwdikr</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Abalone is the pearl/green shift of my dreams</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwdikr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1dwdg3w</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Alright 'ristas, here we go! My Mooncat order arrived unbroken, and the bottles withstood testing. I'm so excited 💃🏻💅🏽 Thanks for all the votes, I chose Venus Flytrap and Garden of Evil, first 💚💖 Scroll for some pics in different lighting! Click in for best view</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwdg3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1dwdbom</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Looking for basecoat recommendations for my 7 year old</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwdbom/looking_for_basecoat_recommendations_for_my_7/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1dwdbmn</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>BKL This is Caelid!</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8dwc49zpsad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1dwceaf</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>How can I get my nails to stop peeling?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i439738nhsad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1dwc8if</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue Verging on Black -Horseshoe Crab Blood is the new Ox Blood </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwc8if</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1dwbzhz</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Craving a good green flakie for this sunny weather (in the garden mystery flakie, Kathleen and co)</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwbzhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1dwbuum</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Sour Note by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/brgj9tf1dsad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1dwbux2</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Where to buy replacement bottles to decant polish into?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwbux2/where_to_buy_replacement_bottles_to_decant_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1dwb7jr</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Thank you to the person who suggested using Psionic as a topper</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y7n75l1t7sad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1dwarqr</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>I made it 24 hours</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwarqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1dwaj66</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Cirque Colors Snow Cone 🩵</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04chl9qc2sad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1dwai0u</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Is jojoba oil the reason my manicures don’t last?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj0vo1r12sad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1dwa877</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>New polish for the collection</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwa877</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1dw802d</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>LynBDesigns - Let’s Bounce!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yri1kdrairad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1dw7g81</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>L.A. Colors in shade lucky with riptide on top</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bctx6u9ydrad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1dw7qjj</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Bummer again</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dw7qjj/bummer_again/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1dw7p0h</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>I love a good green combo 💚</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jipndieqfrad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1dw7lum</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Mooncat email re: broken bottles (3 images)</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw7lum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1dw7ext</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Why have manicurists started going so hard on cuticles?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dw7ext/why_have_manicurists_started_going_so_hard_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1dw71ph</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>My BKL order came in ✨</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw71ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1dw6m01</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Need assistance locating YSL No. 1 Rouge Pop Art as it is currently unavailable.</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dw6m01/need_assistance_locating_ysl_no_1_rouge_pop_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1dw6ibs</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>yum 🌞</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw6ibs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1dvoxq0</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Soak-off products</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvoxq0/soakoff_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1dw69ai</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>I can’t stop staring at my nails!!🤩🤩 felt the need to show them off on here haha :)</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw69ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1dw63ch</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A beautiful polish by Daveen. </t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw63ch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1dw5zzr</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Belated Fourth of July Post</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvaxffaq2rad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1dw5vn9</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>My Cock-a-doodle-doom is way more like a ruby red than a purple with red shimmer. Am I insane or should I contact the seller?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw5vn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1dw58xn</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Last minute mashup &amp; advice needed</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw58xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1dw505s</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Watermelon/Strawberry Nails :)</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2v8iun6vqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1dw4xdw</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>That work bathoom lighting is something else, I tell ya</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlt1smrkuqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1dw4rlc</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>ILNP Mutagen + Essie Shine of the Times</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw4rlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1dw42f0</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Layering Toppers Under Jelly Polish</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/poyk65l1oqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1dw3xhr</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Does anyone know when Ethereal Lacquer opens for PPU rewind?!</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgxg1k40nqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1dw3won</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Pandemonium by Mooncat for the fourth 🧨</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yph9cg3umqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1dw3j8f</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>First gradient using Mooncat x PPG</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13jk1o11kqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1dw2pgh</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Ether Dragon ✨🐉 really is THAT girl</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw2pgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1dw2mli</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Cannot get over the sparkle in this!!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owcgs6f5dqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1dw1oez</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Queer Flag Colors</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw1oez</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1dvzgtc</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>What would I ask for to have this color/texture at the salon?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt4grpdiopad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1dvykm5</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Narf Narf Narf</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxz5tgk6hpad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1dvyco6</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Best way to mix lacquer?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvyco6/best_way_to_mix_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1dvxs34</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Can't get over my love for a transluecent polish with aurora powder on top.</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4gko411iapad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1dvxhv5</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Layering shimmer/glitter over some thermals</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvxhv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1dvx8j0</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>✨️🌈Crushed Holo Gradient🌈✨️</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvx8j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1dvv0r5</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Tangerine, tangerine. Living reflections from a dream... 🍊</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvv0r5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1dvts5a</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decanting/repotting nail polish tips/guides? </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dvts5a/decantingrepotting_nail_polish_tipsguides/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1dwk3wj</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Best top coat for nail art stickers-non gel?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dwk3wj/best_top_coat_for_nail_art_stickersnon_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1dwg1kn</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>I am so excited for the set I am working on!!!😍</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8w8m2kk0gtad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1dwerve</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Summer Strawberry Picnic</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwerve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1dwdtfk</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>First time doing my Nails</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fddw1samusad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1dwcmmv</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Is it too early to give up?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/corh39oojsad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1dwcm23</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>First time using decals!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwcm23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1dwbo4o</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tequila sunrise </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwbo4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1dwa499</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>She has a horror theme birthday party coming up so i did her birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwa499</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1dw98du</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts and tips? </t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsnjzwq2srad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1dw6t9v</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Experimenting with art. First time.</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5pmrpg29rad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1dw657s</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kira from JOJO's bizarre adventure, tutorial/process video link in description </t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw657s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1dw2ida</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Green &amp; black nails</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw2ida</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1dw2hsb</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black and White Anime Nails </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf7sdl25cqad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1dw02vn</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Critique and tips ( Reddit keeps washing out my first picture</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dw02vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1dvxyr3</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>New color</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvxyr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1dvxyn6</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>First attempt at BIAB and a little nail art</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dvxyn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1dvxq77</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>My favorite type of nail art!</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zs1zf713apad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1dvuo9g</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for the Calgary Stampede! </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuhf7lyoeoad1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jul  7 08:08:07 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_07.xlsx
+++ b/data/2024_07_07.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1234"/>
+  <dimension ref="A1:C1406"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21412,6 +21412,2930 @@
         </is>
       </c>
     </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1dx5s23</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Is there anything like this?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fua3bydp90bd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1dx6sww</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very confused on my nail desires </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dx6sww/very_confused_on_my_nail_desires/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1dx9i1h</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>First time getting 3D nail art! I love them so much!</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9eabxfgd1bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1dx8qxx</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Getting engaged soon :) what nail shape/color would be best for me to get?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83cufv6j41bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1dx8h1d</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Still learning the art of at-home gel nails ft. my kiddo!</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s77kdxhg11bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1dx89e7</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>First time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvfzw516z0bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1dx7o6f</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>The joy of finding a good nude color</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nh8bjwnvs0bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1dx7j2a</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Last time I had a ‘too much’ pink set. And I loved them so much I did ‘too much’ blue next!</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx7j2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1dx7db9</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx7db9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1dx7b51</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Nude and Gold Nails</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tw6p1m1p0bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1dx79ye</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Not perfect but I’m getting better</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx79ye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1dx7662</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Which shape looks best on me?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx7662</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1dx75mj</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Wet N Wild- Bubble Gum Pop</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx75mj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1dx756l</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Wet N Wild-Teal or No Teal, going in my destash pile</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx756l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1dx6ka4</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>my wedding nails!</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx6ka4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1dx6hln</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Which shape looks best/ what shape/length would suit me if not either of these?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx6hln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1dx6fss</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I layer OPI nail lacquer like their gel colors? </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dx6fss/can_i_layer_opi_nail_lacquer_like_their_gel_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1dx6eba</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>how do u do this is it just clear acrylic set with clear nail polish and then chrome powder ?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fom9gj7xf0bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1dx6ajr</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Love the color and design I went with but I feel like the pointer finger is way too curved. Am I crazy? 2nd pic for ref.</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx6ajr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1dx60dw</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>So angry I could cry</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx60dw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1dx5zu2</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Finally got around to doing my nails</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx5zu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1dx55aw</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Once upon a time, I spent 3 hours on my nails </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx55aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1dx4uw1</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished my first set on another person! </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kl2f5req00bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1dx4uj3</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Chrome wins again 🩵💙💜</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4b4hruwm00bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1dx4lb4</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50$ refill with design 🌼 </t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njxzain5yzad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1dx4kgm</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Press- ons to the rescue 🦹‍♀️</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx4kgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1dx4hds</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Little press on set I painted for my mum!</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx4hds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1dx4ce7</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Does this look good on my complexion?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx4ce7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1dx49y7</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>I LOVE!!!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fozj2v86vzad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1dx48pv</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>One year without polish and all issues are gone</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7yjj2guuzad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1dx46yv</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>i glued 3 extensions together</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3u52ldduzad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1dx3ppw</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Is it weird that I don't like my natural nails long under sns</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dx3ppw/is_it_weird_that_i_dont_like_my_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1dx3mnf</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Thoughts on new gel mani?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx3mnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1dx3i1c</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>DIY</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rv86a79xnzad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1dx3hz0</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Pink magical sparkling nails ✨🌟💕</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx3hz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1dx3fzt</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Stream Brat 💚 diy gel x jellies</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fybgr8wenzad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1dx3b1r</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time having stiletto nails. Show me your favourite stiletto set. </t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ji86wks7mzad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1dx393i</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Do you like pastel nails?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zseusv4rlzad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1dx34go</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seriously Summer Shorties 💅 </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx34go</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1dx2w4g</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>I got clunky 3D Nails :)</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx2w4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1dx2tpk</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>is it over for me</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx2tpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1dx2oka</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Sometimes , I surprise myself</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crcwx6engzad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1dx28bm</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>I asked my nail tech for pop art nails, and he delivered!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx28bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1dx25qg</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing gel nails </t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro83zxa2czad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1dx1w6x</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>advice for frenchies and making the layers even/smooth?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fve8cjps9zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1dx1vpv</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Happy belated 4th</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5jn1fuo9zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1dx1pg8</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Fresh from the nail salon! #short</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfitl9j78zad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1dx1omw</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Cantarito nails for my client’s baby shower!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx1omw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1dx1mtw</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Fun summer nails ☀️</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivlchp0m7zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1dx1m39</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Routine 🥹🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p705d0vf7zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1dx1k1h</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st dip </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hsr03ky6zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1dx1el4</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>cat eye nails</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx1el4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1dx1bnm</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/965b3i3z4zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1dx17g7</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Harley Davidson 🖤🧡</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5kj37wz3zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1dx110b</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Do these look like iron deficiency?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tifjy4mi2zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1dx0zhn</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Some sets I’ve had this year 🥰</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx0zhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1dwzy2j</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They like the combination </t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbld9a1mtyad1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1dwzhbd</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Chrome Watercolor</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s4lg6zrpyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1dwzg20</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Apex check</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwzg20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1dwzcqq</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silk wrap overlay for strength? </t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dwzcqq/silk_wrap_overlay_for_strength/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1dwzbk5</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Fruity 🍋🍊🥝</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03l7kxygoyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1dwzanf</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want your berries ... </t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u43q8pz8oyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1dwz6l6</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>First time trying Chrome Powder!</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0sm6s4bnyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1dwz5ty</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>SNS dip w/tips + chrome done @salon. Are they uneven?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zr0yd6w4nyad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1dwyybz</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wzh46bflyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1dwyvek</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>What form of nails would be best for me?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qjxpdhqkyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1dwyhr7</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Heeelp! E-file not working</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hguj3nlhyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1dwygmj</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>My nails so far this year !!</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwygmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1dwygk1</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>What price should I put on this type of design?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmk7i2lbhyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1dwyehx</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Trial &amp; Error…but I did it!</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwyehx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1dwxv6f</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Just did my own nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwxv6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1dwxuuf</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>The only instruction she gave me was the color(purple)</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwxuuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1dwxmsn</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Squoval or oval?</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwxmsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1dwxd0n</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Me expressed as a color 🧡</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltz60s4f8yad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1dwx2f4</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with this nail color </t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6po5a7666yad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1dwx0x6</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>what nail shape is this??</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6euavpgu5yad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1dwwsc3</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time doing press ons </t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwwsc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1dwwqlm</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Do you ever do gel AND regular nail polish?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dwwqlm/do_you_ever_do_gel_and_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1dwwq3c</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>The video just really captures the effect better than pics. Sound on for bonus "moooom" from my toddler. 🥰</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ehu937ph3yad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1dwwpts</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Treat for myself</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cwn7e7g3yad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1dwwjxn</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>I love gel polish on my toes!</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwwjxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1dwwgwt</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>I have stubby fingers and nail beds…how to make them look good?</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwwgwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1dwwfk7</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>🍃💨💨 Sanrio!</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wdtsa851yad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1dwwc3a</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>In a nail rut!</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwwc3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1dww3ts</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Nail stamping plates</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dww3ts/nail_stamping_plates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1dww208</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Patriotic but understated</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dww208</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1dwvy1f</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need major cuticle care help )): </t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwvy1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1dwvtne</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i got chrome nails for the first time and i'm OBSESSED </t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwvtne</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1dwvsm7</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Todays client. She was supershy, but i think she liked them</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en4b0yiuvxad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1dwvm95</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Kinda sad to get a new set- love my pride nails</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt5y2mahuxad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1dwvbfb</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>I’ve finished the first hand</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwvbfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1dwvay2</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Lines In Nails??</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwvay2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1dwva7m</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>PPG here to save my nails</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwva7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1dwv9ha</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>I'm on summer break and my current fixation is deciding which mani/pedi colors to get for vacation. I went so far as creating color schemes but would love some input. I'd like to for sure have a red coral color but can't choose what to pair it with!</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwv9ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1dwv8b8</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tell me if you love it! Ido! </t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h41g48vdrxad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1dwv7e9</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Fresh summer set this morning :)</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3xhkln5rxad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1dwv3vc</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Did my friends nails last night. Took me 3 hrs but it was so fun!!</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwv3vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1dwv1fm</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>In my Ultra Fem Era</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a9cp3jtpxad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1dwuzpf</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>I’m trying to stay away from solid colors and stiletto/almond shapes! What’re we thinking ladies?</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl9xqbigpxad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1dwuk0z</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>I'm literally so obsessed with these</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwuk0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1dxacl3</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Mooncat Millenia</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dxacl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1dx9pf3</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">music festival nails </t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx9pf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1dx82nf</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>OPI - Infinite Shine: On Cloud Fine</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx82nf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1dx7dsm</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nails pop off within hours or a day of applying. What do I do? </t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dx7dsm/gel_nails_pop_off_within_hours_or_a_day_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1dx6llu</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>My stumbly bumbly bees</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx6llu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1dx61c3</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nail strip help </t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dx61c3/gel_nail_strip_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1dx5y3q</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Manicure catch up!</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx5y3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1dx5tpu</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer!!!✨✨✨</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx5tpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1dx5ezb</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Mercury in Retrograde</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx5ezb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1dx4h2u</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>I got gel polish on my skin and I’m freaking out!</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dx4h2u/i_got_gel_polish_on_my_skin_and_im_freaking_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1dx3lha</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>I'm Too Pretty To Mess With</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx3lha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1dx31kl</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Summer makes me crave watermelon</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx31kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1dx2x8y</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>I wanted something bright 😎</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx2x8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1dx2w0f</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>What type of nails should I try next?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dx2w0f/what_type_of_nails_should_i_try_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1dx2six</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Jior - The Doc Is In (June 2024 PPU)</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ebz90imlhzad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1dx27lm</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Love this color combo</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx27lm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1dx1ycf</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>back to an old fav 💋 (Essie - Berry Naughty)</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx1ycf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1dx1eai</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Kathleen &amp; co - Gravity Falls June 2024 PPU</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d59h4jol5zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1dx1340</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Moonwalk </t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx1340</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1dx0wnz</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>I’ve been playing with a clip on macro lens on my phone… and I can see my neighbor’s red house and white roof in my nails 😵‍💫</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmyoflbj1zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1dx0ie5</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Anyone know of any dupes for Cirque Tiny Dancer?</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dx0ie5/anyone_know_of_any_dupes_for_cirque_tiny_dancer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1dx052u</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to get a fully opaque creme? </t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzfg5d08vyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1dwzx7z</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>My nails match my favourite mug!</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwzx7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1dwxcrb</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Mooncat Mani + Customer service</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwxcrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1dwzeq3</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Thoughts on Dazzle Dry “Pinkies Up” manicure?</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jmn5ud7pyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1dwyvb5</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Starry sky inspired ✨</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dvht5qpkyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1dwxrr7</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>A shape that begs for multichrome lacquer...</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9fqee6wbyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1dwxps3</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Torrent 👻🐎</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwxps3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1dwxbrg</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>How do I stop my pinkie nail from chipping?</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1dlb1p98yad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1dwxagi</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>What causes these bubbles?</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8rkef4z7yad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1dwwqhd</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Hello, it's me</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vweqdcnl3yad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1dwwdwd</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Hitsuzen</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwwdwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1dwwaff</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>🎶Let’s get dangerous🎶</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwwaff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1dww7k0</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Here is your sign to layer random shit and see what happens </t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xci7ve77zxad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1dww6qe</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Hazbin Hotel mani</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dww6qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1dww1ql</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>I know I was literally *just* on here, but I honestly think Garden of Evil is one of my top favorite shades that I've ever owned. LOOK @ HER 💚💖</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87vxj6awxxad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1dwvxbp</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can i used just base coat and top coat on the base coat? </t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwvxbp/can_i_used_just_base_coat_and_top_coat_on_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1dwvr9n</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>I think I subconsciously picked a rock that matched my nails</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f7lbc3rivxad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1dwvjwp</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>I’ll just be over here eating my own words</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwvjwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1dwvch4</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Orchid 💐</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uewu681csxad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1dwv3ma</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>❤️⚡️Red Ranger⚡️❤️</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwv3ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1dwum9t</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>ILNP 'Lily' is the most beautiful polish ever</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3p9r3z4imxad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1dwul78</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Happy 5th Birthday to Holo Taco!!</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwul78</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1dws8wv</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>This colour is 100% worth the hype - 10/10, would recommend.</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dws8wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1dwsyx6</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Wanted summery, ended up Halloweeny 🤣</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7z7bp5r59xad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1dwsd4l</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>First time wearing Lurid 🔥</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwsd4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1dwscy0</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>DVN Tomato Plant in a Gully</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9v4imx94xad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1dwsai9</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Does anybody else skip out on top coat?</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j877owhp3xad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1dwrkzd</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Scofflaw Varnish out of business?</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwrkzd/scofflaw_varnish_out_of_business/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1dwr85u</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Is Ethereal Lacquer “the best” for ethereal type polishes?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwr85u/is_ethereal_lacquer_the_best_for_ethereal_type/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1dwqp60</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Londontown nail veil as a base for jellies, toppers, polishes?</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dwqp60/londontown_nail_veil_as_a_base_for_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1dwq94c</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>MC’s Mercury In Retrograde - silver shimmer magnetic dupe?</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c3o7pbxmwad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1dwq6o1</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Day 1 vs. Day 17 of my Holo Taco gradient</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwq6o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1dwpxix</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy with my new indie polishes </t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwpxix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1dwpip4</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>LynB can do no wrong and I am OBSESSED</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwpip4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1dwpf26</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>BNL Let’s See The Stars/ILNP Flower Child</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q8vui8ofwad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1dwoxom</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Mercury 🫧</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwoxom</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1dwouj1</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Swatching became an unintentional skittle</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwouj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1dx90d3</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>First go at 3d solid sculpting gel.</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/si1h4m0l71bd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1dx870m</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Cat eye💋</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/np9oj8gfy0bd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1dx7f6z</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Berries 🍓🫐🍇</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx7f6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1dx4f1y</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freehand french tip </t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dx4f1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1dx2mz3</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Love when this happens &lt;3</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pqzo9bx7gzad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1dx1mos</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>I like to combine</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp4kwvxk7zad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1dwzdl6</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Recent Festival Nails </t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmfy3wbyoyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1dwzdi9</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Nails Bae Gold Chrome Powder Set. You Like ? </t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqu9niqxoyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1dwzcue</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Fruity 🍋🍊🥝</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qeyv1zuroyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1dwzcjw</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>I want your berries ...</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0ucyfipoyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1dwynaw</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>A msg from snoopy 💨</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7yswapuiyad1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1dwyeoe</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>I am editing the bts of this set let me know if you want to see more!🖤</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p3bvy7nvgyad1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1dwv4ju</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Looking for a transparent red shifting nail powder</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dwv4ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1dwfafz</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Recent set</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qhfsbjm8tad1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>